<commit_message>
Modified avl tree and bst algorithm
modify and delete replicated python file
</commit_message>
<xml_diff>
--- a/experiment table.xlsx
+++ b/experiment table.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+  <si>
+    <t xml:space="preserve">Experiment Type: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVL Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operation:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insertion</t>
+  </si>
   <si>
     <t xml:space="preserve">Time Taken to execute</t>
   </si>
@@ -28,21 +43,26 @@
     <t xml:space="preserve">Dataset</t>
   </si>
   <si>
-    <t xml:space="preserve">Average</t>
+    <t xml:space="preserve">Average BST Insertion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average AVL Insertion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -61,56 +81,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Lohit Devanagari"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -124,57 +95,15 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -182,23 +111,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -222,73 +136,51 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB3B3B3"/>
@@ -300,7 +192,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -316,16 +208,16 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFD320"/>
+      <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -338,7 +230,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -381,32 +273,32 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$2</c:f>
+              <c:f>Sheet1!$L$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average</c:v>
+                  <c:v>Average BST Insertion</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="ffd320"/>
+              <a:srgbClr val="004586"/>
             </a:solidFill>
             <a:ln w="28800">
               <a:solidFill>
-                <a:srgbClr val="ffd320"/>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="triangle"/>
+            <c:symbol val="square"/>
             <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ffd320"/>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
@@ -420,77 +312,198 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:f>Sheet1!$A$5:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900000</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10000000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$3:$L$12</c:f>
+              <c:f>Sheet1!$L$5:$L$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5.6965</c:v>
+                  <c:v>1.039</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.0895</c:v>
+                  <c:v>2.3627</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.8056</c:v>
+                  <c:v>3.9244</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.8644</c:v>
+                  <c:v>5.2204</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.2556</c:v>
+                  <c:v>7.0833</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.8943</c:v>
+                  <c:v>8.4687</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42.3172</c:v>
+                  <c:v>11.1459</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>46.2536</c:v>
+                  <c:v>12.8873</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52.3873</c:v>
+                  <c:v>15.6286</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>56.9315</c:v>
+                  <c:v>17.3471</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Y$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average AVL Insertion</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$5:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Y$5:$Y$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.4313</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.168</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0131</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.343</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.9012</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.6808</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.6749</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.2361</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25.0079</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29.4733</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -505,11 +518,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="58359995"/>
-        <c:axId val="5866307"/>
+        <c:axId val="6961448"/>
+        <c:axId val="45224546"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58359995"/>
+        <c:axId val="6961448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -565,14 +578,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5866307"/>
+        <c:crossAx val="45224546"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5866307"/>
+        <c:axId val="45224546"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -615,7 +628,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -637,7 +650,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58359995"/>
+        <c:crossAx val="6961448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -689,16 +702,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>69120</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>413640</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>492480</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>124560</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>30960</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -706,8 +719,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="69120" y="2151720"/>
-        <a:ext cx="7828560" cy="4475160"/>
+        <a:off x="3870360" y="2656800"/>
+        <a:ext cx="8254800" cy="4474440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -725,469 +738,923 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="6.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.1"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.81"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="16" style="0" width="6.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="12.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="B2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>2</v>
+      <c r="N2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>5.343</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>6.457</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>6.716</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>4.838</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>6.819</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>5.147</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>4.32</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>5.448</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>6.567</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>5.31</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <f aca="false">SUM(B3:K3)/10</f>
-        <v>5.6965</v>
-      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="O3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>2000000</v>
+    <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>11.237</v>
+        <v>1</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>12.512</v>
+        <v>2</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>11.712</v>
+        <v>3</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>9.515</v>
+        <v>4</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>11.661</v>
+        <v>5</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>10.587</v>
+        <v>6</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>8.655</v>
+        <v>7</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>11.333</v>
+        <v>8</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>14.649</v>
+        <v>9</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>9.034</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <f aca="false">SUM(B4:K4)/10</f>
-        <v>11.0895</v>
+        <v>10</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>3000000</v>
+        <v>100000</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>16.705</v>
+        <v>0.902</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>16.732</v>
+        <v>0.976</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>16.049</v>
+        <v>0.974</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>17.328</v>
+        <v>0.966</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>16.553</v>
+        <v>1.038</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>12.208</v>
+        <v>1.137</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>14.037</v>
+        <v>1.153</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>16.728</v>
+        <v>1.062</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>13.246</v>
+        <v>1.067</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>18.47</v>
+        <v>1.115</v>
       </c>
       <c r="L5" s="0" t="n">
         <f aca="false">SUM(B5:K5)/10</f>
-        <v>15.8056</v>
+        <v>1.039</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>100000</v>
+      </c>
+      <c r="O5" s="4" t="n">
+        <v>2.184</v>
+      </c>
+      <c r="P5" s="4" t="n">
+        <v>2.645</v>
+      </c>
+      <c r="Q5" s="4" t="n">
+        <v>2.502</v>
+      </c>
+      <c r="R5" s="4" t="n">
+        <v>2.419</v>
+      </c>
+      <c r="S5" s="4" t="n">
+        <v>2.294</v>
+      </c>
+      <c r="T5" s="4" t="n">
+        <v>2.387</v>
+      </c>
+      <c r="U5" s="4" t="n">
+        <v>2.667</v>
+      </c>
+      <c r="V5" s="4" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="W5" s="4" t="n">
+        <v>2.415</v>
+      </c>
+      <c r="X5" s="4" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="Y5" s="4" t="n">
+        <f aca="false">SUM(O5:X5)/10</f>
+        <v>2.4313</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>4000000</v>
+        <v>200000</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>23.473</v>
+        <v>2.117</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>24.162</v>
+        <v>2.295</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>18.268</v>
+        <v>2.372</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>21.604</v>
+        <v>2.55</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>19.171</v>
+        <v>2.406</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>23.458</v>
+        <v>2.412</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>24.415</v>
+        <v>2.62</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>19.151</v>
+        <v>2.293</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>27.242</v>
+        <v>2.298</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>17.7</v>
+        <v>2.264</v>
       </c>
       <c r="L6" s="0" t="n">
         <f aca="false">SUM(B6:K6)/10</f>
-        <v>21.8644</v>
+        <v>2.3627</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>200000</v>
+      </c>
+      <c r="O6" s="4" t="n">
+        <v>4.985</v>
+      </c>
+      <c r="P6" s="4" t="n">
+        <v>5.324</v>
+      </c>
+      <c r="Q6" s="4" t="n">
+        <v>5.35</v>
+      </c>
+      <c r="R6" s="4" t="n">
+        <v>5.251</v>
+      </c>
+      <c r="S6" s="4" t="n">
+        <v>5.207</v>
+      </c>
+      <c r="T6" s="4" t="n">
+        <v>5.159</v>
+      </c>
+      <c r="U6" s="4" t="n">
+        <v>4.938</v>
+      </c>
+      <c r="V6" s="4" t="n">
+        <v>5.238</v>
+      </c>
+      <c r="W6" s="4" t="n">
+        <v>5.163</v>
+      </c>
+      <c r="X6" s="4" t="n">
+        <v>5.065</v>
+      </c>
+      <c r="Y6" s="4" t="n">
+        <f aca="false">SUM(O6:X6)/10</f>
+        <v>5.168</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>5000000</v>
+        <v>300000</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>31.246</v>
+        <v>3.742</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>28.043</v>
+        <v>4.134</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>27.962</v>
+        <v>3.819</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>26.153</v>
+        <v>4.185</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>24.838</v>
+        <v>4.008</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>23.773</v>
+        <v>3.785</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>28.022</v>
+        <v>3.879</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>22.669</v>
+        <v>3.889</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>34.356</v>
+        <v>3.806</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>15.494</v>
+        <v>3.997</v>
       </c>
       <c r="L7" s="0" t="n">
         <f aca="false">SUM(B7:K7)/10</f>
-        <v>26.2556</v>
+        <v>3.9244</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>300000</v>
+      </c>
+      <c r="O7" s="4" t="n">
+        <v>7.843</v>
+      </c>
+      <c r="P7" s="4" t="n">
+        <v>8.069</v>
+      </c>
+      <c r="Q7" s="4" t="n">
+        <v>8.101</v>
+      </c>
+      <c r="R7" s="4" t="n">
+        <v>8.272</v>
+      </c>
+      <c r="S7" s="4" t="n">
+        <v>8.014</v>
+      </c>
+      <c r="T7" s="4" t="n">
+        <v>7.972</v>
+      </c>
+      <c r="U7" s="4" t="n">
+        <v>7.927</v>
+      </c>
+      <c r="V7" s="4" t="n">
+        <v>7.956</v>
+      </c>
+      <c r="W7" s="4" t="n">
+        <v>7.977</v>
+      </c>
+      <c r="X7" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y7" s="4" t="n">
+        <f aca="false">SUM(O7:X7)/10</f>
+        <v>8.0131</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>6000000</v>
+        <v>400000</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>35.067</v>
+        <v>5.143</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>32.587</v>
+        <v>5.378</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>35.52</v>
+        <v>5.327</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>24.353</v>
+        <v>5.139</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>27.747</v>
+        <v>5.168</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>35.319</v>
+        <v>5.114</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>29.742</v>
+        <v>5.341</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>36.957</v>
+        <v>5.221</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>30.143</v>
+        <v>5.247</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>41.508</v>
+        <v>5.126</v>
       </c>
       <c r="L8" s="0" t="n">
         <f aca="false">SUM(B8:K8)/10</f>
-        <v>32.8943</v>
+        <v>5.2204</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>400000</v>
+      </c>
+      <c r="O8" s="4" t="n">
+        <v>10.558</v>
+      </c>
+      <c r="P8" s="4" t="n">
+        <v>11.658</v>
+      </c>
+      <c r="Q8" s="4" t="n">
+        <v>11.514</v>
+      </c>
+      <c r="R8" s="4" t="n">
+        <v>11.281</v>
+      </c>
+      <c r="S8" s="4" t="n">
+        <v>11.175</v>
+      </c>
+      <c r="T8" s="4" t="n">
+        <v>11.633</v>
+      </c>
+      <c r="U8" s="4" t="n">
+        <v>11.582</v>
+      </c>
+      <c r="V8" s="4" t="n">
+        <v>11.32</v>
+      </c>
+      <c r="W8" s="4" t="n">
+        <v>11.312</v>
+      </c>
+      <c r="X8" s="4" t="n">
+        <v>11.397</v>
+      </c>
+      <c r="Y8" s="4" t="n">
+        <f aca="false">SUM(O8:X8)/10</f>
+        <v>11.343</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>7000000</v>
+        <v>500000</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>40.434</v>
+        <v>7.024</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>40.897</v>
+        <v>7.256</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>41.499</v>
+        <v>7.559</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>46.113</v>
+        <v>6.981</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>43.626</v>
+        <v>7.396</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>26.257</v>
+        <v>6.945</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>48.089</v>
+        <v>7.04</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>49.094</v>
+        <v>6.975</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>34.097</v>
+        <v>6.819</v>
       </c>
       <c r="K9" s="0" t="n">
-        <v>53.066</v>
+        <v>6.838</v>
       </c>
       <c r="L9" s="0" t="n">
         <f aca="false">SUM(B9:K9)/10</f>
-        <v>42.3172</v>
+        <v>7.0833</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>500000</v>
+      </c>
+      <c r="O9" s="4" t="n">
+        <v>13.655</v>
+      </c>
+      <c r="P9" s="4" t="n">
+        <v>13.77</v>
+      </c>
+      <c r="Q9" s="4" t="n">
+        <v>13.959</v>
+      </c>
+      <c r="R9" s="4" t="n">
+        <v>13.681</v>
+      </c>
+      <c r="S9" s="4" t="n">
+        <v>13.879</v>
+      </c>
+      <c r="T9" s="4" t="n">
+        <v>14.023</v>
+      </c>
+      <c r="U9" s="4" t="n">
+        <v>14.086</v>
+      </c>
+      <c r="V9" s="4" t="n">
+        <v>14.016</v>
+      </c>
+      <c r="W9" s="4" t="n">
+        <v>13.995</v>
+      </c>
+      <c r="X9" s="4" t="n">
+        <v>13.948</v>
+      </c>
+      <c r="Y9" s="4" t="n">
+        <f aca="false">SUM(O9:X9)/10</f>
+        <v>13.9012</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>8000000</v>
+        <v>600000</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>49.537</v>
+        <v>8.214</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>48.475</v>
+        <v>8.52</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>45.214</v>
+        <v>8.494</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>44.933</v>
+        <v>8.62</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>41.979</v>
+        <v>8.349</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>43.121</v>
+        <v>8.478</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>50.724</v>
+        <v>8.646</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>40.031</v>
+        <v>8.308</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>58.93</v>
+        <v>8.471</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>39.592</v>
+        <v>8.587</v>
       </c>
       <c r="L10" s="0" t="n">
         <f aca="false">SUM(B10:K10)/10</f>
-        <v>46.2536</v>
+        <v>8.4687</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>600000</v>
+      </c>
+      <c r="O10" s="4" t="n">
+        <v>16.472</v>
+      </c>
+      <c r="P10" s="4" t="n">
+        <v>16.591</v>
+      </c>
+      <c r="Q10" s="4" t="n">
+        <v>16.833</v>
+      </c>
+      <c r="R10" s="4" t="n">
+        <v>17.041</v>
+      </c>
+      <c r="S10" s="4" t="n">
+        <v>16.195</v>
+      </c>
+      <c r="T10" s="4" t="n">
+        <v>16.442</v>
+      </c>
+      <c r="U10" s="4" t="n">
+        <v>16.857</v>
+      </c>
+      <c r="V10" s="4" t="n">
+        <v>16.596</v>
+      </c>
+      <c r="W10" s="4" t="n">
+        <v>16.723</v>
+      </c>
+      <c r="X10" s="4" t="n">
+        <v>17.058</v>
+      </c>
+      <c r="Y10" s="4" t="n">
+        <f aca="false">SUM(O10:X10)/10</f>
+        <v>16.6808</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>9000000</v>
+        <v>700000</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>45.785</v>
+        <v>11.161</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>51.685</v>
+        <v>12.135</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>50.073</v>
+        <v>10.965</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>58.141</v>
+        <v>11.334</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>52.445</v>
+        <v>11.404</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>42.89</v>
+        <v>10.472</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>60.542</v>
+        <v>11.191</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>54.31</v>
+        <v>11.356</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>37.41</v>
+        <v>10.874</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>70.592</v>
+        <v>10.567</v>
       </c>
       <c r="L11" s="0" t="n">
         <f aca="false">SUM(B11:K11)/10</f>
-        <v>52.3873</v>
+        <v>11.1459</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>700000</v>
+      </c>
+      <c r="O11" s="4" t="n">
+        <v>18.943</v>
+      </c>
+      <c r="P11" s="4" t="n">
+        <v>20.846</v>
+      </c>
+      <c r="Q11" s="4" t="n">
+        <v>20.888</v>
+      </c>
+      <c r="R11" s="4" t="n">
+        <v>20.731</v>
+      </c>
+      <c r="S11" s="4" t="n">
+        <v>21.088</v>
+      </c>
+      <c r="T11" s="4" t="n">
+        <v>20.881</v>
+      </c>
+      <c r="U11" s="4" t="n">
+        <v>21.094</v>
+      </c>
+      <c r="V11" s="4" t="n">
+        <v>20.614</v>
+      </c>
+      <c r="W11" s="4" t="n">
+        <v>21.059</v>
+      </c>
+      <c r="X11" s="4" t="n">
+        <v>20.605</v>
+      </c>
+      <c r="Y11" s="4" t="n">
+        <f aca="false">SUM(O11:X11)/10</f>
+        <v>20.6749</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>10000000</v>
+        <v>800000</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>56.409</v>
+        <v>11.846</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>60.423</v>
+        <v>12.442</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>61.328</v>
+        <v>12.285</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>58.21</v>
+        <v>12.633</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>57.793</v>
+        <v>13.137</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>60.705</v>
+        <v>12.473</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>65.131</v>
+        <v>13.425</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>32.86</v>
+        <v>13.731</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>69.322</v>
+        <v>14.229</v>
       </c>
       <c r="K12" s="0" t="n">
-        <v>47.134</v>
+        <v>12.672</v>
       </c>
       <c r="L12" s="0" t="n">
         <f aca="false">SUM(B12:K12)/10</f>
-        <v>56.9315</v>
+        <v>12.8873</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>800000</v>
+      </c>
+      <c r="O12" s="4" t="n">
+        <v>21.592</v>
+      </c>
+      <c r="P12" s="4" t="n">
+        <v>23.99</v>
+      </c>
+      <c r="Q12" s="4" t="n">
+        <v>23.031</v>
+      </c>
+      <c r="R12" s="4" t="n">
+        <v>22.939</v>
+      </c>
+      <c r="S12" s="4" t="n">
+        <v>22.82</v>
+      </c>
+      <c r="T12" s="4" t="n">
+        <v>23.861</v>
+      </c>
+      <c r="U12" s="4" t="n">
+        <v>22.901</v>
+      </c>
+      <c r="V12" s="4" t="n">
+        <v>23.092</v>
+      </c>
+      <c r="W12" s="4" t="n">
+        <v>23.844</v>
+      </c>
+      <c r="X12" s="4" t="n">
+        <v>24.291</v>
+      </c>
+      <c r="Y12" s="4" t="n">
+        <f aca="false">SUM(O12:X12)/10</f>
+        <v>23.2361</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>900000</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>15.284</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>16.319</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>15.88</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>15.185</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>14.791</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>15.618</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>16.043</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>15.301</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>15.412</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>16.453</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <f aca="false">SUM(B13:K13)/10</f>
+        <v>15.6286</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>900000</v>
+      </c>
+      <c r="O13" s="4" t="n">
+        <v>23.53</v>
+      </c>
+      <c r="P13" s="4" t="n">
+        <v>25.873</v>
+      </c>
+      <c r="Q13" s="4" t="n">
+        <v>25.247</v>
+      </c>
+      <c r="R13" s="4" t="n">
+        <v>25.829</v>
+      </c>
+      <c r="S13" s="4" t="n">
+        <v>24.621</v>
+      </c>
+      <c r="T13" s="4" t="n">
+        <v>24.868</v>
+      </c>
+      <c r="U13" s="4" t="n">
+        <v>24.936</v>
+      </c>
+      <c r="V13" s="4" t="n">
+        <v>24.771</v>
+      </c>
+      <c r="W13" s="4" t="n">
+        <v>25.679</v>
+      </c>
+      <c r="X13" s="4" t="n">
+        <v>24.725</v>
+      </c>
+      <c r="Y13" s="4" t="n">
+        <f aca="false">SUM(O13:X13)/10</f>
+        <v>25.0079</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>17.155</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>18.193</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>19.338</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>18.189</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>16.858</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>16.457</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>16.649</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>16.285</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>16.43</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>17.917</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <f aca="false">SUM(B14:K14)/10</f>
+        <v>17.3471</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="O14" s="4" t="n">
+        <v>28.353</v>
+      </c>
+      <c r="P14" s="4" t="n">
+        <v>31.03</v>
+      </c>
+      <c r="Q14" s="4" t="n">
+        <v>32.21</v>
+      </c>
+      <c r="R14" s="4" t="n">
+        <v>30.688</v>
+      </c>
+      <c r="S14" s="4" t="n">
+        <v>29.406</v>
+      </c>
+      <c r="T14" s="4" t="n">
+        <v>28.677</v>
+      </c>
+      <c r="U14" s="4" t="n">
+        <v>28.622</v>
+      </c>
+      <c r="V14" s="4" t="n">
+        <v>28.553</v>
+      </c>
+      <c r="W14" s="4" t="n">
+        <v>28.57</v>
+      </c>
+      <c r="X14" s="4" t="n">
+        <v>28.624</v>
+      </c>
+      <c r="Y14" s="4" t="n">
+        <f aca="false">SUM(O14:X14)/10</f>
+        <v>29.4733</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:L1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="O3:Y3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>